<commit_message>
Reduce tolerances by half
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33772EC3-0759-4447-9E1A-0E0E34DE54DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18A756ED-7795-4584-9D79-3106A934B91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J5 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J3 J4 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K3 K5 K4 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L3 L5 L4 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add offset cycloidal disc config
The two discs should be asymmetrical. The gearbox now meshes correctly.
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18A756ED-7795-4584-9D79-3106A934B91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{51E68A6B-BB4D-4A20-B35C-56BEA9136DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>$VALUE@eccentricity@EQUATIONS</t>
   </si>
   <si>
-    <t>=ROUND ( ("pin_pitch_dia" / 2) / "N_pins" * 0.7 , 2 )</t>
-  </si>
-  <si>
     <t>=0.1mm</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>=("pin_pitch_dia" / 2) / "N_pins" * 0.7</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>11</v>
@@ -492,13 +492,13 @@
         <v>14</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
@@ -524,7 +524,7 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -536,7 +536,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
@@ -548,16 +548,16 @@
         <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -583,7 +583,7 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -595,7 +595,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
@@ -607,21 +607,21 @@
         <v>7</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -633,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>3</v>
@@ -645,21 +645,21 @@
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -671,7 +671,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -683,27 +683,27 @@
         <v>7</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J3 J4 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K3 K5 K4 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L3 L5 L4 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Tolerance motor brackets & leg assy
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51E68A6B-BB4D-4A20-B35C-56BEA9136DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D22325EE-B398-4D26-B8F7-FFFC1A027F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="veryHidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Replace output plate shaft with removable shaft
Also, correct tolerance stackup on rotor adaptor ring & groove
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D22325EE-B398-4D26-B8F7-FFFC1A027F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5C5E1F6-C9D4-46D5-8BAF-93BCC1E3965C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Enable rotation of the gearbox
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5C5E1F6-C9D4-46D5-8BAF-93BCC1E3965C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9076C76C-022B-41E6-BF98-E587E63FC517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update leg assy with (SpeedPak'd) motor module.
Since the motors are SpeedPak'd, the hip and splay remain inflexible for
now
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9076C76C-022B-41E6-BF98-E587E63FC517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EF28B06-3F40-4EAD-9096-3D6124438F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Create chassis w/ battery, odrives, etc
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E984934-ABA5-4605-9888-865650A7C9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{131CB2E8-AE26-47FD-9878-9461DB4ECBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix mates on hex shafts
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4079AECF-581D-4B6A-8197-2F74169529FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F18F91C-6ED8-472C-9514-F78A551632BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="veryHidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Split motor module housing into 2 pieces
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F18F91C-6ED8-472C-9514-F78A551632BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04DB40BB-B029-4C7A-ABCF-9039EDF3B6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>$STATE@6294K444_Dry-Running MDS-Filled Nylon Sleeve Bearing&lt;1&gt;</t>
   </si>
   <si>
-    <t>$STATE@LocalCirPattern4</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>=("pin_pitch_dia" / 2) / "N_pins" * 0.7</t>
+  </si>
+  <si>
+    <t>$STATE@Cycloidal Roller Bushings Pattern</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -498,7 +498,7 @@
         <v>24</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
@@ -548,16 +548,16 @@
         <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -607,16 +607,16 @@
         <v>7</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -645,16 +645,16 @@
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -683,27 +683,27 @@
         <v>7</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@LocalCirPattern4" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Flip bolt alignment between motor & gearbox casings
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04DB40BB-B029-4C7A-ABCF-9039EDF3B6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D50B830-4E2C-4690-8729-9B6B82272284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J3 J5 J4 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K3 K5 K4 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Extend motor module to accomodate encoder wires
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D50B830-4E2C-4690-8729-9B6B82272284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E743D37B-85F7-4BC0-AA78-00B4628EB1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J3 J5 J4 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K3 K5 K4 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L3 L5 L4 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Reduce encoder cable clearance by 5mm
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E743D37B-85F7-4BC0-AA78-00B4628EB1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD47D190-048C-4B6D-AD2F-B35EC26DAABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Replace AMT103 encoder & mount with wide-base
Also fixed hole dias for joining the motor & gearbox casings
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD47D190-048C-4B6D-AD2F-B35EC26DAABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDA5F926-EF0D-4C4C-BD37-62B133E5296F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L3 L5 L4 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update motor module tols
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4737A93-052B-47F2-98A6-F3FF7D5B0A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65D3E949-58F6-414B-9257-06BEE2695FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -697,13 +697,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L3 L5 L4 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Merge rotor adaptor ring and adaptor
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59CFAC48-95BC-4D0F-8D97-885749ACFA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BF9AF4D-1EAC-46A1-9D0A-FE6FB0D2BFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -700,13 +700,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update pin dia and tols
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDF64501-7C3A-4D93-A8F7-6722B25E8380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59CFAC48-95BC-4D0F-8D97-885749ACFA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t/>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>$STATE@Cycloidal Roller Bushings Pattern</t>
+  </si>
+  <si>
+    <t>=6.375mm</t>
   </si>
 </sst>
 </file>
@@ -542,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>7</v>
@@ -601,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>7</v>
@@ -639,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>7</v>
@@ -677,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>7</v>
@@ -703,7 +706,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Split motor casing into 2 parts
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6F2F42F-63B5-460C-83E6-AB91271F96BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0E63C75-689F-4B12-B145-EB9FFF944C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -703,13 +703,13 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings,Bearings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3" xr:uid="{5C11469F-3D7B-4565-A3EF-2FD8DB96E4A6}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3" xr:uid="{20FD32EB-0AE6-4601-953E-E6BC6383F7A7}">
       <formula1>"With Bushings,No Bushings,Bearings"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update assembly & output shaft
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BF9AF4D-1EAC-46A1-9D0A-FE6FB0D2BFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6F2F42F-63B5-460C-83E6-AB91271F96BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="28665" yWindow="-30" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="veryHidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -699,15 +699,18 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J4 J3 J5 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
-      <formula1>"With Bushings,No Bushings"</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+      <formula1>"With Bushings,No Bushings,Bearings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3" xr:uid="{5C11469F-3D7B-4565-A3EF-2FD8DB96E4A6}">
+      <formula1>"With Bushings,No Bushings,Bearings"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>

<commit_message>
Enbeefen output shaft pin holes
</commit_message>
<xml_diff>
--- a/q-pup/motor_module/cycloidal_params.xlsx
+++ b/q-pup/motor_module/cycloidal_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0E63C75-689F-4B12-B145-EB9FFF944C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3C05C9F-D8CB-41B5-8C05-DA44CC97A9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView visibility="veryHidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -699,18 +699,15 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
+  <dataValidations count="3">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3 J2" xr:uid="{C4DD3C0F-3C08-467A-9078-8853F064FD6A}">
       <formula1>"With Bushings,No Bushings,Bearings"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K4 K3 K5 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@6294K444_Dry-Running MDS-" prompt="Select to suppress or resolve the component_x000a_Possible Options:_x000a_Suppressed_x000a_Resolved_x000a_S = Suppressed_x000a_R = Resolved_x000a_1 = Suppressed_x000a_0 = Resolved" sqref="K5 K4 K3 K2" xr:uid="{2ED1CFF0-5CB5-4516-B5E8-179472A37733}">
       <formula1>"SUPPRESSED,RESOLVED,S,R,1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L4 L3 L5 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$STATE@Cycloidal Roller Bushings" prompt="Select to suppress or unsuppress the feature_x000a_Possible Options:_x000a_Suppressed_x000a_Unsuppressed_x000a_S = Suppressed_x000a_U = Unsuppressed_x000a_1 = Suppressed_x000a_0 = Unsuppressed" sqref="L5 L4 L3 L2" xr:uid="{6DCCA65E-B6EC-4A8D-8E9C-60EE7E5B0335}">
       <formula1>"SUPPRESSED,UNSUPPRESSED,S,U,1,0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="$CONFIGURATION@output_shaft&lt;1&gt;" prompt="Select the configuration name." sqref="J5 J4 J3" xr:uid="{20FD32EB-0AE6-4601-953E-E6BC6383F7A7}">
-      <formula1>"With Bushings,No Bushings,Bearings"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>